<commit_message>
Starting to work on unit 5.1
</commit_message>
<xml_diff>
--- a/SpringBoard_Timeline.xlsx
+++ b/SpringBoard_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abulh\Sync\Documents\O4_P1_SpringBoardMLCourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C5752F-D9ED-4533-B25D-A6DF9319EC92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C203B766-8343-4D49-9751-D402AF317713}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="983" yWindow="-98" windowWidth="19634" windowHeight="13875" activeTab="1" xr2:uid="{E81A3A76-C87B-4E26-A2EB-FC8CEC27FB4E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Days</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Days per</t>
+  </si>
+  <si>
+    <t>&lt;- Come back to as needed</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1CF0EB-18BA-4EE2-B849-8C4B87D88420}">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -426,32 +429,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>43647</v>
+        <v>43657</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>43648</v>
+        <v>43658</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>43649</v>
+        <v>43659</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -459,10 +462,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>43650</v>
+        <v>43660</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -470,10 +473,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>43651</v>
+        <v>43661</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -481,10 +484,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>43652</v>
+        <v>43662</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -492,10 +495,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
-        <v>43653</v>
+        <v>43663</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -503,10 +506,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
-        <v>43654</v>
+        <v>43664</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -514,10 +517,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>43655</v>
+        <v>43665</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -525,10 +528,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
-        <v>43656</v>
+        <v>43666</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -536,10 +539,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
-        <v>43657</v>
+        <v>43667</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -547,10 +550,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>43658</v>
+        <v>43668</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -558,10 +561,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
-        <v>43659</v>
+        <v>43669</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -569,10 +572,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
-        <v>43660</v>
+        <v>43670</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -580,10 +583,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
-        <v>43661</v>
+        <v>43671</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -591,10 +594,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
-        <v>43662</v>
+        <v>43672</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -602,10 +605,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1">
-        <v>43663</v>
+        <v>43673</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -613,10 +616,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1">
-        <v>43664</v>
+        <v>43674</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -624,10 +627,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1">
-        <v>43665</v>
+        <v>43675</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -635,10 +638,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1">
-        <v>43666</v>
+        <v>43676</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -646,10 +649,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
-        <v>43667</v>
+        <v>43677</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -657,10 +660,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
-        <v>43668</v>
+        <v>43678</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -668,10 +671,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1">
-        <v>43669</v>
+        <v>43679</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -679,10 +682,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
-        <v>43670</v>
+        <v>43680</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -690,10 +693,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1">
-        <v>43671</v>
+        <v>43681</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -701,10 +704,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1">
-        <v>43672</v>
+        <v>43682</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -712,10 +715,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
-        <v>43673</v>
+        <v>43683</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -723,10 +726,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1">
-        <v>43674</v>
+        <v>43684</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -734,10 +737,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1">
-        <v>43675</v>
+        <v>43685</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -745,10 +748,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
-        <v>43676</v>
+        <v>43686</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -756,10 +759,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1">
-        <v>43677</v>
+        <v>43687</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -767,10 +770,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1">
-        <v>43678</v>
+        <v>43688</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -778,10 +781,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1">
-        <v>43679</v>
+        <v>43689</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -789,10 +792,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1">
-        <v>43680</v>
+        <v>43690</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -800,10 +803,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1">
-        <v>43681</v>
+        <v>43691</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -811,10 +814,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1">
-        <v>43682</v>
+        <v>43692</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -822,10 +825,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1">
-        <v>43683</v>
+        <v>43693</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -833,10 +836,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1">
-        <v>43684</v>
+        <v>43694</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -844,10 +847,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1">
-        <v>43685</v>
+        <v>43695</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -855,10 +858,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1">
-        <v>43686</v>
+        <v>43696</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -866,10 +869,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B42" s="1">
-        <v>43687</v>
+        <v>43697</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -877,10 +880,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B43" s="1">
-        <v>43688</v>
+        <v>43698</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -888,10 +891,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1">
-        <v>43689</v>
+        <v>43699</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -899,10 +902,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1">
-        <v>43690</v>
+        <v>43700</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -910,10 +913,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1">
-        <v>43691</v>
+        <v>43701</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -921,10 +924,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B47" s="1">
-        <v>43692</v>
+        <v>43702</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -932,10 +935,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1">
-        <v>43693</v>
+        <v>43703</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -943,10 +946,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B49" s="1">
-        <v>43694</v>
+        <v>43704</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -954,10 +957,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1">
-        <v>43695</v>
+        <v>43705</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -965,10 +968,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1">
-        <v>43696</v>
+        <v>43706</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -976,10 +979,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B52" s="1">
-        <v>43697</v>
+        <v>43707</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -987,10 +990,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B53" s="1">
-        <v>43698</v>
+        <v>43708</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -998,10 +1001,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B54" s="1">
-        <v>43699</v>
+        <v>43709</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1009,10 +1012,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1">
-        <v>43700</v>
+        <v>43710</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1020,10 +1023,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B56" s="1">
-        <v>43701</v>
+        <v>43711</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1031,10 +1034,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B57" s="1">
-        <v>43702</v>
+        <v>43712</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1042,10 +1045,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B58" s="1">
-        <v>43703</v>
+        <v>43713</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1053,10 +1056,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B59" s="1">
-        <v>43704</v>
+        <v>43714</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1064,10 +1067,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B60" s="1">
-        <v>43705</v>
+        <v>43715</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1075,10 +1078,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B61" s="1">
-        <v>43706</v>
+        <v>43716</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1086,10 +1089,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B62" s="1">
-        <v>43707</v>
+        <v>43717</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1097,10 +1100,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B63" s="1">
-        <v>43708</v>
+        <v>43718</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1108,10 +1111,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B64" s="1">
-        <v>43709</v>
+        <v>43719</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1119,10 +1122,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B65" s="1">
-        <v>43710</v>
+        <v>43720</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1130,10 +1133,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1">
-        <v>43711</v>
+        <v>43721</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1141,10 +1144,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B67" s="1">
-        <v>43712</v>
+        <v>43722</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -1152,10 +1155,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1">
-        <v>43713</v>
+        <v>43723</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1163,10 +1166,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B69" s="1">
-        <v>43714</v>
+        <v>43724</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1174,10 +1177,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1">
-        <v>43715</v>
+        <v>43725</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -1185,10 +1188,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1">
-        <v>43716</v>
+        <v>43726</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -1196,10 +1199,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B72" s="1">
-        <v>43717</v>
+        <v>43727</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1207,10 +1210,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B73" s="1">
-        <v>43718</v>
+        <v>43728</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1218,10 +1221,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B74" s="1">
-        <v>43719</v>
+        <v>43729</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B75" s="1">
-        <v>43720</v>
+        <v>43730</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -1240,10 +1243,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B76" s="1">
-        <v>43721</v>
+        <v>43731</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -1251,10 +1254,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B77" s="1">
-        <v>43722</v>
+        <v>43732</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -1262,10 +1265,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B78" s="1">
-        <v>43723</v>
+        <v>43733</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -1273,10 +1276,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B79" s="1">
-        <v>43724</v>
+        <v>43734</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -1284,10 +1287,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B80" s="1">
-        <v>43725</v>
+        <v>43735</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -1295,10 +1298,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B81" s="1">
-        <v>43726</v>
+        <v>43736</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -1306,10 +1309,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B82" s="1">
-        <v>43727</v>
+        <v>43737</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1317,10 +1320,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B83" s="1">
-        <v>43728</v>
+        <v>43738</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -1328,10 +1331,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B84" s="1">
-        <v>43729</v>
+        <v>43739</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -1339,10 +1342,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B85" s="1">
-        <v>43730</v>
+        <v>43740</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -1350,10 +1353,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B86" s="1">
-        <v>43731</v>
+        <v>43741</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -1361,10 +1364,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B87" s="1">
-        <v>43732</v>
+        <v>43742</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -1372,10 +1375,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B88" s="1">
-        <v>43733</v>
+        <v>43743</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -1383,10 +1386,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B89" s="1">
-        <v>43734</v>
+        <v>43744</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -1394,10 +1397,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B90" s="1">
-        <v>43735</v>
+        <v>43745</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -1405,10 +1408,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B91" s="1">
-        <v>43736</v>
+        <v>43746</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -1416,10 +1419,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1">
-        <v>43737</v>
+        <v>43747</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -1427,10 +1430,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1">
-        <v>43738</v>
+        <v>43748</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -1438,10 +1441,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B94" s="1">
-        <v>43739</v>
+        <v>43749</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -1449,10 +1452,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B95" s="1">
-        <v>43740</v>
+        <v>43750</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -1460,10 +1463,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1">
-        <v>43741</v>
+        <v>43751</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -1471,10 +1474,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B97" s="1">
-        <v>43742</v>
+        <v>43752</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -1482,10 +1485,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B98" s="1">
-        <v>43743</v>
+        <v>43753</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -1493,10 +1496,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B99" s="1">
-        <v>43744</v>
+        <v>43754</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -1504,10 +1507,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B100" s="1">
-        <v>43745</v>
+        <v>43755</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -1515,10 +1518,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B101" s="1">
-        <v>43746</v>
+        <v>43756</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -1526,10 +1529,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B102" s="1">
-        <v>43747</v>
+        <v>43757</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -1537,10 +1540,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B103" s="1">
-        <v>43748</v>
+        <v>43758</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -1548,10 +1551,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B104" s="1">
-        <v>43749</v>
+        <v>43759</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -1559,10 +1562,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B105" s="1">
-        <v>43750</v>
+        <v>43760</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -1570,10 +1573,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B106" s="1">
-        <v>43751</v>
+        <v>43761</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -1581,10 +1584,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B107" s="1">
-        <v>43752</v>
+        <v>43762</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -1592,10 +1595,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B108" s="1">
-        <v>43753</v>
+        <v>43763</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -1603,10 +1606,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B109" s="1">
-        <v>43754</v>
+        <v>43764</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -1614,10 +1617,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B110" s="1">
-        <v>43755</v>
+        <v>43765</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -1625,10 +1628,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B111" s="1">
-        <v>43756</v>
+        <v>43766</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -1636,10 +1639,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B112" s="1">
-        <v>43757</v>
+        <v>43767</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -1647,10 +1650,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B113" s="1">
-        <v>43758</v>
+        <v>43768</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -1658,10 +1661,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B114" s="1">
-        <v>43759</v>
+        <v>43769</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -1669,10 +1672,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B115" s="1">
-        <v>43760</v>
+        <v>43770</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -1680,10 +1683,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B116" s="1">
-        <v>43761</v>
+        <v>43771</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -1691,10 +1694,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B117" s="1">
-        <v>43762</v>
+        <v>43772</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -1702,10 +1705,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B118" s="1">
-        <v>43763</v>
+        <v>43773</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -1713,10 +1716,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1">
-        <v>43764</v>
+        <v>43774</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -1724,10 +1727,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B120" s="1">
-        <v>43765</v>
+        <v>43775</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -1735,10 +1738,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1">
-        <v>43766</v>
+        <v>43776</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -1746,10 +1749,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1">
-        <v>43767</v>
+        <v>43777</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -1757,10 +1760,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1">
-        <v>43768</v>
+        <v>43778</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -1768,10 +1771,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B124" s="1">
-        <v>43769</v>
+        <v>43779</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -1779,10 +1782,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B125" s="1">
-        <v>43770</v>
+        <v>43780</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -1790,10 +1793,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B126" s="1">
-        <v>43771</v>
+        <v>43781</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -1801,10 +1804,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B127" s="1">
-        <v>43772</v>
+        <v>43782</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -1812,10 +1815,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B128" s="1">
-        <v>43773</v>
+        <v>43783</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -1823,10 +1826,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B129" s="1">
-        <v>43774</v>
+        <v>43784</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -1834,10 +1837,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B130" s="1">
-        <v>43775</v>
+        <v>43785</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -1845,10 +1848,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B131" s="1">
-        <v>43776</v>
+        <v>43786</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -1856,10 +1859,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B132" s="1">
-        <v>43777</v>
+        <v>43787</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -1867,10 +1870,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B133" s="1">
-        <v>43778</v>
+        <v>43788</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -1878,10 +1881,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B134" s="1">
-        <v>43779</v>
+        <v>43789</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -1889,10 +1892,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B135" s="1">
-        <v>43780</v>
+        <v>43790</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -1900,10 +1903,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B136" s="1">
-        <v>43781</v>
+        <v>43791</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -1911,10 +1914,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B137" s="1">
-        <v>43782</v>
+        <v>43792</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -1922,10 +1925,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B138" s="1">
-        <v>43783</v>
+        <v>43793</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -1933,10 +1936,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B139" s="1">
-        <v>43784</v>
+        <v>43794</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -1944,10 +1947,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B140" s="1">
-        <v>43785</v>
+        <v>43795</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -1955,10 +1958,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B141" s="1">
-        <v>43786</v>
+        <v>43796</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -1966,10 +1969,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B142" s="1">
-        <v>43787</v>
+        <v>43797</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -1977,10 +1980,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B143" s="1">
-        <v>43788</v>
+        <v>43798</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -1988,10 +1991,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B144" s="1">
-        <v>43789</v>
+        <v>43799</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -1999,10 +2002,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B145" s="1">
-        <v>43790</v>
+        <v>43800</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2010,10 +2013,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B146" s="1">
-        <v>43791</v>
+        <v>43801</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -2021,10 +2024,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B147" s="1">
-        <v>43792</v>
+        <v>43802</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -2032,10 +2035,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B148" s="1">
-        <v>43793</v>
+        <v>43803</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -2043,10 +2046,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B149" s="1">
-        <v>43794</v>
+        <v>43804</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2054,10 +2057,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B150" s="1">
-        <v>43795</v>
+        <v>43805</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -2065,10 +2068,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B151" s="1">
-        <v>43796</v>
+        <v>43806</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2076,10 +2079,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B152" s="1">
-        <v>43797</v>
+        <v>43807</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -2087,10 +2090,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B153" s="1">
-        <v>43798</v>
+        <v>43808</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2098,10 +2101,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B154" s="1">
-        <v>43799</v>
+        <v>43809</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -2109,10 +2112,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B155" s="1">
-        <v>43800</v>
+        <v>43810</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2120,10 +2123,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B156" s="1">
-        <v>43801</v>
+        <v>43811</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -2131,10 +2134,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B157" s="1">
-        <v>43802</v>
+        <v>43812</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2142,10 +2145,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B158" s="1">
-        <v>43803</v>
+        <v>43813</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -2153,10 +2156,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B159" s="1">
-        <v>43804</v>
+        <v>43814</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2164,10 +2167,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B160" s="1">
-        <v>43805</v>
+        <v>43815</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -2175,129 +2178,19 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161">
+        <v>170</v>
+      </c>
+      <c r="B161" s="1">
+        <v>43816</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C162">
+        <f>SUM(C2:C161)</f>
         <v>160</v>
-      </c>
-      <c r="B161" s="1">
-        <v>43806</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A162">
-        <v>161</v>
-      </c>
-      <c r="B162" s="1">
-        <v>43807</v>
-      </c>
-      <c r="C162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A163">
-        <v>162</v>
-      </c>
-      <c r="B163" s="1">
-        <v>43808</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A164">
-        <v>163</v>
-      </c>
-      <c r="B164" s="1">
-        <v>43809</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A165">
-        <v>164</v>
-      </c>
-      <c r="B165" s="1">
-        <v>43810</v>
-      </c>
-      <c r="C165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A166">
-        <v>165</v>
-      </c>
-      <c r="B166" s="1">
-        <v>43811</v>
-      </c>
-      <c r="C166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A167">
-        <v>166</v>
-      </c>
-      <c r="B167" s="1">
-        <v>43812</v>
-      </c>
-      <c r="C167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A168">
-        <v>167</v>
-      </c>
-      <c r="B168" s="1">
-        <v>43813</v>
-      </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A169">
-        <v>168</v>
-      </c>
-      <c r="B169" s="1">
-        <v>43814</v>
-      </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A170">
-        <v>169</v>
-      </c>
-      <c r="B170" s="1">
-        <v>43815</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A171">
-        <v>170</v>
-      </c>
-      <c r="B171" s="1">
-        <v>43816</v>
-      </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C172">
-        <f>SUM(C2:C171)</f>
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2307,10 +2200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB10BD22-4D96-4E87-8235-21A9365626A8}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2319,7 +2212,7 @@
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2333,7 +2226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2351,7 +2244,7 @@
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2369,25 +2262,28 @@
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>COMPLETE</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2405,7 +2301,7 @@
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2423,7 +2319,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2441,7 +2337,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2459,7 +2355,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2477,7 +2373,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2495,7 +2391,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2513,7 +2409,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2531,7 +2427,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2549,7 +2445,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2567,7 +2463,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2585,7 +2481,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2678,7 +2574,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21">
         <f>SUM(B2:B20)</f>
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:D21" si="1">SUM(C2:C20)</f>
@@ -2686,21 +2582,21 @@
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>511</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B22">
-        <f>B21/Sheet1!$C$172</f>
-        <v>0.54761904761904767</v>
+        <f>B21/Sheet1!$C$162</f>
+        <v>0.53749999999999998</v>
       </c>
       <c r="C22">
-        <f>C21/Sheet1!$C$172</f>
-        <v>0.19642857142857142</v>
+        <f>C21/Sheet1!$C$162</f>
+        <v>0.20624999999999999</v>
       </c>
       <c r="D22">
-        <f>(D21/Sheet1!$C$172)*1.5</f>
-        <v>4.5625</v>
+        <f>(D21/Sheet1!$C$162)*1.5</f>
+        <v>4.5187500000000007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -2709,11 +2605,11 @@
       </c>
       <c r="B23">
         <f>1/B22</f>
-        <v>1.826086956521739</v>
+        <v>1.8604651162790697</v>
       </c>
       <c r="C23">
         <f t="shared" ref="C23" si="2">1/C22</f>
-        <v>5.0909090909090908</v>
+        <v>4.8484848484848486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>